<commit_message>
new mobile testing project
</commit_message>
<xml_diff>
--- a/Test_Documentation/Checklists/Web_app/Checklists_for_learn.epam.com_STA_course.xlsx
+++ b/Test_Documentation/Checklists/Web_app/Checklists_for_learn.epam.com_STA_course.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lilia\Documents\I-Tester_Portfolio\Portfolio_Tester\Test_Documentation\Checklists\Web_app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1E62DFD-9FAC-4E68-9FCF-41DDE4027988}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{970485F1-D3CD-451C-B191-94B53022BF9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37770" yWindow="-3800" windowWidth="37770" windowHeight="20360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38510" yWindow="-4430" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Checklist learn.epam.com" sheetId="1" r:id="rId1"/>
@@ -613,9 +613,6 @@
     <t>II. Checklists for Non-Functional Testing of learn.epam.com (on March 2023)</t>
   </si>
   <si>
-    <t>I. Checklists for Functionality of learn.epam.com (on March 2023)</t>
-  </si>
-  <si>
     <t>The reason for the need for smoke or regression testing</t>
   </si>
   <si>
@@ -672,7 +669,10 @@
     <t>The button "Send" the message works correctly.</t>
   </si>
   <si>
-    <t>Back on main page</t>
+    <t>Back on the main page</t>
+  </si>
+  <si>
+    <t>I. Checklists for Functionality of learn.epam.com (on April 2023)</t>
   </si>
 </sst>
 </file>
@@ -700,39 +700,45 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="9" tint="0.79998168889431442"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -978,8 +984,8 @@
     <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1044,8 +1050,8 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1366,7 +1372,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H1" sqref="H1"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1383,8 +1389,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="H1" s="57" t="s">
-        <v>202</v>
+      <c r="H1" s="35" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -1401,7 +1407,7 @@
         <v>7</v>
       </c>
       <c r="E2" s="34" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F2" s="34" t="s">
         <v>8</v>
@@ -1410,12 +1416,12 @@
         <v>9</v>
       </c>
       <c r="H2" s="33" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="42" t="s">
-        <v>185</v>
+        <v>202</v>
       </c>
       <c r="B3" s="42"/>
       <c r="C3" s="42"/>
@@ -1430,7 +1436,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="39" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C4" s="39"/>
       <c r="D4" s="39"/>
@@ -1448,7 +1454,7 @@
         <v>6</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="10" t="s">
@@ -1486,7 +1492,7 @@
       <c r="B7" s="38"/>
       <c r="C7" s="37"/>
       <c r="D7" s="12" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="29" t="s">
@@ -1496,7 +1502,7 @@
         <v>11</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="94.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -1648,7 +1654,7 @@
         <v>11</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1658,7 +1664,7 @@
       <c r="B16" s="38"/>
       <c r="C16" s="37"/>
       <c r="D16" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="10" t="s">
@@ -1866,7 +1872,7 @@
         <v>6</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E27" s="3"/>
       <c r="F27" s="10" t="s">
@@ -1904,7 +1910,7 @@
       <c r="B29" s="38"/>
       <c r="C29" s="37"/>
       <c r="D29" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E29" s="2"/>
       <c r="F29" s="29" t="s">
@@ -1914,7 +1920,7 @@
         <v>11</v>
       </c>
       <c r="H29" s="53" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1924,7 +1930,7 @@
       <c r="B30" s="38"/>
       <c r="C30" s="37"/>
       <c r="D30" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E30" s="2"/>
       <c r="F30" s="29" t="s">
@@ -2008,7 +2014,7 @@
         <v>11</v>
       </c>
       <c r="H34" s="7" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -2054,7 +2060,7 @@
         <v>6</v>
       </c>
       <c r="D37" s="25" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E37" s="3"/>
       <c r="F37" s="10" t="s">
@@ -2438,7 +2444,7 @@
         <v>92</v>
       </c>
       <c r="B58" s="39" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C58" s="39"/>
       <c r="D58" s="39"/>
@@ -2512,7 +2518,7 @@
       <c r="B62" s="38"/>
       <c r="C62" s="37"/>
       <c r="D62" s="26" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E62" s="3"/>
       <c r="F62" s="10" t="s">
@@ -2608,7 +2614,7 @@
         <v>104</v>
       </c>
       <c r="B68" s="39" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C68" s="39"/>
       <c r="D68" s="39"/>
@@ -2970,7 +2976,7 @@
         <v>142</v>
       </c>
       <c r="B88" s="39" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C88" s="39"/>
       <c r="D88" s="39"/>
@@ -3054,9 +3060,10 @@
       </c>
     </row>
     <row r="95" spans="1:8" ht="72" x14ac:dyDescent="0.3">
-      <c r="B95" s="35" t="s">
-        <v>202</v>
-      </c>
+      <c r="B95" s="57" t="s">
+        <v>201</v>
+      </c>
+      <c r="C95" s="57"/>
       <c r="E95" s="21"/>
       <c r="F95" s="10"/>
       <c r="G95" s="6" t="s">
@@ -3089,7 +3096,8 @@
       <c r="G102" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="72">
+  <mergeCells count="73">
+    <mergeCell ref="B95:C95"/>
     <mergeCell ref="F93:H93"/>
     <mergeCell ref="B90:H90"/>
     <mergeCell ref="H44:H48"/>
@@ -3164,8 +3172,8 @@
     <mergeCell ref="B19:B25"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B95" r:id="rId1" xr:uid="{20CAD1C3-6D87-46FA-9061-9B6B6860129B}"/>
-    <hyperlink ref="H1" r:id="rId2" xr:uid="{C1729FE9-EA40-456C-B48C-E02DC50D67A7}"/>
+    <hyperlink ref="B95" r:id="rId1" display="Back on main page" xr:uid="{20CAD1C3-6D87-46FA-9061-9B6B6860129B}"/>
+    <hyperlink ref="H1" r:id="rId2" display="Back on main page" xr:uid="{C1729FE9-EA40-456C-B48C-E02DC50D67A7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>

</xml_diff>